<commit_message>
created excel files and marked videos
</commit_message>
<xml_diff>
--- a/data/df_videos_2020.xlsx
+++ b/data/df_videos_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzobehna/projects/Social-Computing_Final-Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uzh-my.sharepoint.com/personal/ishwarya_sutharsan_uzh_ch/Documents/Desktop/Uni/Uni_ZH/Computerlinguistik/6_Semester/Social_Computing/Project_Git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23DB2938-8900-C145-A239-8C75D6D0C36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{23DB2938-8900-C145-A239-8C75D6D0C36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5F4EF5-BBC8-4497-A80B-606850ABBBEC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{85C328E1-DADD-0A42-A214-062159DE5668}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{85C328E1-DADD-0A42-A214-062159DE5668}"/>
   </bookViews>
   <sheets>
     <sheet name="df_videos_2020" sheetId="1" r:id="rId1"/>
@@ -1364,63 +1364,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1436,7 +1428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1755,53 +1747,53 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.6875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1823,7 +1815,7 @@
       <c r="G2" s="2">
         <v>21378</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -1836,7 +1828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1858,7 +1850,7 @@
       <c r="G3" s="2">
         <v>4987</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1871,7 +1863,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1893,7 +1885,7 @@
       <c r="G4" s="2">
         <v>3007</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1906,7 +1898,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1928,7 +1920,7 @@
       <c r="G5" s="2">
         <v>1727</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1941,72 +1933,74 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>2990743</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>1870</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>27</v>
       </c>
+      <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="e">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="e">
         <f>-ePZ7OdY-Dw</f>
         <v>#NAME?</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>2857676</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>2226</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>27</v>
       </c>
+      <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
@@ -2028,7 +2022,7 @@
       <c r="G8" s="2">
         <v>1679</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -2041,7 +2035,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
@@ -2063,7 +2057,7 @@
       <c r="G9" s="2">
         <v>995</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -2076,39 +2070,40 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>1631987</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>5455</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>10</v>
       </c>
+      <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>72</v>
       </c>
@@ -2130,7 +2125,7 @@
       <c r="G11" s="2">
         <v>665</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -2143,232 +2138,239 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>1090028</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>570</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>28</v>
       </c>
+      <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>742652</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>1182</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>28</v>
       </c>
+      <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="e">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A14" s="1" t="e">
         <f>-g0xOJYPjkQ</f>
         <v>#NAME?</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>387935</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>548</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>22</v>
       </c>
+      <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>374354</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>1077</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
         <v>28</v>
       </c>
+      <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>356476</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>1167</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <v>27</v>
       </c>
+      <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>304453</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>753</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>27</v>
       </c>
+      <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>299913</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>767</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>27</v>
       </c>
+      <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>126</v>
       </c>
@@ -2390,7 +2392,7 @@
       <c r="G19" s="2">
         <v>1055</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>131</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -2399,8 +2401,9 @@
       <c r="J19" s="2">
         <v>27</v>
       </c>
+      <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>133</v>
       </c>
@@ -2422,7 +2425,7 @@
       <c r="G20" s="2">
         <v>1048</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>138</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -2431,8 +2434,9 @@
       <c r="J20" s="2">
         <v>24</v>
       </c>
+      <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>139</v>
       </c>
@@ -2454,7 +2458,7 @@
       <c r="G21" s="2">
         <v>802</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>144</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -2463,6 +2467,7 @@
       <c r="J21" s="2">
         <v>22</v>
       </c>
+      <c r="K21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>